<commit_message>
Added buttons, aux power distribution and connections to PI Pico
</commit_message>
<xml_diff>
--- a/E-ink-Pico-BOM.xlsx
+++ b/E-ink-Pico-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t xml:space="preserve">Part ID</t>
   </si>
@@ -34,10 +34,16 @@
     <t xml:space="preserve">Price</t>
   </si>
   <si>
+    <t xml:space="preserve">Totals</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Link</t>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouser</t>
   </si>
   <si>
     <t xml:space="preserve">Alternate</t>
@@ -127,7 +133,7 @@
     <t xml:space="preserve">DMP2045U-7DICT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Power Select Transistor</t>
+    <t xml:space="preserve">Power Select P-Channel MOSFET</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Inc</t>
@@ -137,6 +143,147 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mouser.com/ProductDetail/Diodes-Incorporated/DMP2045U-7/?qs=%2Fha2pyFaduiijUdf5azNaJO26YcbUiF9shg3NLqs7u5clMhkiK5h7w%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC5211-LXYM6-TR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dual Output LDO Voltage Regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/microchip-technology/MIC5211-LXYM6-TR/1616946?s=N4IgTCBcDaILIEkDCBWMBGdBaAMgDQE04A2LAFQCUQBdAXyA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Microchip-Technology-Micrel/MIC5211-LXYM6-TR?qs=U6T8BxXiZAWZW72McTiFRQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lipo Battery 3.7v 2500mAh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Adafruit/328/?qs=%2Fha2pyFadujwErubcL2L61P2WtCOdI0NVdDECC%252B%2FoCOknOIs%252BWOAti9IV6ILMtMSHsGVAGjMTyxRM15aoZcNPEjv2R0X%2FExV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTST-C171KRKT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED RED CLEAR SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lite-On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KRKT/386801?s=N4IgTCBcDaIIwDYAMBaOAWMB2NKByAIiALoC%2BQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KRKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXsqEUEEyi4%2FkmrG730tSpETf1y5CrReP0g%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTST-C171KSKT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED YELLOW CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KSKT/386803?s=N4IgTCBcDaIIwDYAMBaOAWMAONKByAIiALoC%2BQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KSKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXn8t9EMk8utzJwNadB3tUNYbTGxiFNDL%252BQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTST-C171KGKT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED GREEN CLEAR SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KGKT/386799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KGKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXtuidLnLhtS%252BLcjo%252B7rsZImYs2WRq48j3g%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBR0530T3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schottky Diode 0.5A, 30V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/on-semiconductor/MBR0530T3G/1477144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/ON-Semiconductor/MBR0530T3G/?qs=3JMERSakebpEmdUS6GetdQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRLML0100TRPBF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infineon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/infineon-technologies/IRLML0100TRPBF/2202214?s=N4IgTCBcDaIJICUAyBZJAGAjO9AVBACgEIBiAwrgLQByAIiALoC%2BQA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Infineon-IR/IRLML0100TRPBF/?qs=%2Fha2pyFadugzSi28VWDL%252B%2Fj%2FX3doh67wE%2FvCgh7X2pqnmkMc%252Bq1ivg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1825232-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/TE-Connectivity/1825232-1/?qs=sGAEpiMZZMsqIr59i2oRcon9IvqasVjyMHmjVc2ktR8%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSMSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tactile Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/TE-Connectivity-Alcoswitch/FSMSM/?qs=sGAEpiMZZMsqIr59i2oRcuc2r3r3LjiLHQssz2WjmiQ%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFSC1515AHER100M01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/IFSC1515AHER100M01/541-1406-1-ND/2744259?itemSeq=353770760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Dale/IFSC1515AHER100M01/?qs=%2Fha2pyFaduhyEPNk9r%2F290OYvS9yrkIBzEVVa6IllFEq60qCq9iyWQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVQ-P7J01P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90deg Tactile Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Panasonic/EVQ-P7J01P/?qs=sGAEpiMZZMsqIr59i2oRcgbPjJcuopmxlBtPLe3n9e0%3D</t>
   </si>
 </sst>
 </file>
@@ -145,13 +292,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-409][$$]#,##0.00;[RED]\-[$$]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -173,25 +321,34 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -228,41 +385,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -274,6 +443,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -282,21 +511,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:AMJ29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="8.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="19.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,7 +542,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -321,7 +551,12 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AME1" s="1"/>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="AMF1" s="1"/>
       <c r="AMG1" s="1"/>
       <c r="AMH1" s="1"/>
@@ -330,10 +565,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
@@ -341,62 +576,78 @@
       <c r="D2" s="5" t="n">
         <v>64.99</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
+      <c r="E2" s="5" t="n">
+        <f aca="false">D2*C2</f>
+        <v>64.99</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="5" t="n">
         <v>2.92</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="5" t="n">
+        <f aca="false">D3*C3</f>
+        <v>2.92</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>19</v>
+        <v>1.99</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">D4*C4</f>
+        <v>1.99</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>20</v>
+      <c r="A5" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
@@ -404,19 +655,24 @@
       <c r="D5" s="2" t="n">
         <v>0.53</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">D5*C5</f>
+        <v>0.53</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
@@ -424,22 +680,26 @@
       <c r="D6" s="2" t="n">
         <v>1.78</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="E6" s="5" t="n">
+        <f aca="false">D6*C6</f>
+        <v>1.78</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
@@ -447,22 +707,26 @@
       <c r="D7" s="2" t="n">
         <v>0.59</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="5" t="n">
+        <f aca="false">D7*C7</f>
+        <v>0.59</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="G7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>34</v>
+      <c r="A8" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
@@ -470,29 +734,343 @@
       <c r="D8" s="2" t="n">
         <v>0.47</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="5" t="n">
+        <f aca="false">D8*C8</f>
+        <v>0.47</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <f aca="false">D9*C9</f>
+        <v>0.77</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">D10*C10</f>
+        <v>14.95</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <f aca="false">D11*C11</f>
+        <v>0.28</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <f aca="false">D12*C12</f>
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <f aca="false">D13*C13</f>
+        <v>0.28</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <f aca="false">D14*C14</f>
+        <v>0.99</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <f aca="false">D15*C15</f>
+        <v>0.48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <f aca="false">D16*C16</f>
+        <v>0.35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <f aca="false">D17*C17</f>
+        <v>1.89</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <f aca="false">D18*C18</f>
+        <v>0.56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <f aca="false">D19*C19</f>
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="4" t="n">
+        <f aca="false">SUM(E2:E28)</f>
+        <v>94.42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://www.waveshare.com/wiki/7.5inch_e-Paper_HAT"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://www.digikey.in/product-detail/en/w%C3%BCrth-elektronik/693071010811/732-3819-1-ND/3124603"/>
-    <hyperlink ref="G3" r:id="rId3" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/693071010811/?qs=%2Fha2pyFadug2rnWaYGULYHsNDGPBmR35gMiIpGARpbOOgsh6ohipJw%3D%3D"/>
-    <hyperlink ref="F4" r:id="rId4" display="https://www.microcenter.com/product/632771/pico?src=raspberrypi"/>
-    <hyperlink ref="F5" r:id="rId5" display="https://www.digikey.in/product-detail/en/jst-sales-america-inc/S2B-PH-SM4-TB-LF-SN/455-1749-1-ND/926846"/>
-    <hyperlink ref="F6" r:id="rId6" display="https://www.digikey.com/en/products/detail/hirose-electric-co-ltd/FH12A-24S-0-5SH-55/966386"/>
-    <hyperlink ref="G6" r:id="rId7" display="https://www.mouser.com/ProductDetail/Hirose-Connector/FH12A-24S-05SH55/?qs=%2Fha2pyFaduhBL9Ra9C9JJo9wVmxbvHTxvQYdc0zFc5HpowawelgM75Z1xbHioLdK"/>
-    <hyperlink ref="F7" r:id="rId8" display="https://www.digikey.com/en/products/detail/microchip-technology/MCP73831T-2ACI-OT/964301"/>
-    <hyperlink ref="G7" r:id="rId9" display="https://www.mouser.com/ProductDetail/Microchip-Technology/MCP73831T-2ACI-OT/?qs=%2Fha2pyFadug7ns3NDcZ1%252BguMEttpm87FnqDgwUSDURWu9uo0PeBXyw%3D%3D"/>
-    <hyperlink ref="F8" r:id="rId10" display="https://www.digikey.in/products/en?keywords=DMP2045U-7DICT-ND"/>
-    <hyperlink ref="G8" r:id="rId11" display="https://www.mouser.com/ProductDetail/Diodes-Incorporated/DMP2045U-7/?qs=%2Fha2pyFaduiijUdf5azNaJO26YcbUiF9shg3NLqs7u5clMhkiK5h7w%3D%3D"/>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.waveshare.com/wiki/7.5inch_e-Paper_HAT"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://www.digikey.in/product-detail/en/w%C3%BCrth-elektronik/693071010811/732-3819-1-ND/3124603"/>
+    <hyperlink ref="H3" r:id="rId3" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/693071010811/?qs=%2Fha2pyFadug2rnWaYGULYHsNDGPBmR35gMiIpGARpbOOgsh6ohipJw%3D%3D"/>
+    <hyperlink ref="I4" r:id="rId4" display="https://www.microcenter.com/product/632771/pico?src=raspberrypi"/>
+    <hyperlink ref="G5" r:id="rId5" display="https://www.digikey.in/product-detail/en/jst-sales-america-inc/S2B-PH-SM4-TB-LF-SN/455-1749-1-ND/926846"/>
+    <hyperlink ref="G6" r:id="rId6" display="https://www.digikey.com/en/products/detail/hirose-electric-co-ltd/FH12A-24S-0-5SH-55/966386"/>
+    <hyperlink ref="H6" r:id="rId7" display="https://www.mouser.com/ProductDetail/Hirose-Connector/FH12A-24S-05SH55/?qs=%2Fha2pyFaduhBL9Ra9C9JJo9wVmxbvHTxvQYdc0zFc5HpowawelgM75Z1xbHioLdK"/>
+    <hyperlink ref="G7" r:id="rId8" display="https://www.digikey.com/en/products/detail/microchip-technology/MCP73831T-2ACI-OT/964301"/>
+    <hyperlink ref="H7" r:id="rId9" display="https://www.mouser.com/ProductDetail/Microchip-Technology/MCP73831T-2ACI-OT/?qs=%2Fha2pyFadug7ns3NDcZ1%252BguMEttpm87FnqDgwUSDURWu9uo0PeBXyw%3D%3D"/>
+    <hyperlink ref="G8" r:id="rId10" display="https://www.digikey.in/products/en?keywords=DMP2045U-7DICT-ND"/>
+    <hyperlink ref="H8" r:id="rId11" display="https://www.mouser.com/ProductDetail/Diodes-Incorporated/DMP2045U-7/?qs=%2Fha2pyFaduiijUdf5azNaJO26YcbUiF9shg3NLqs7u5clMhkiK5h7w%3D%3D"/>
+    <hyperlink ref="G9" r:id="rId12" display="https://www.digikey.com/en/products/detail/microchip-technology/MIC5211-LXYM6-TR/1616946?s=N4IgTCBcDaILIEkDCBWMBGdBaAMgDQE04A2LAFQCUQBdAXyA"/>
+    <hyperlink ref="H9" r:id="rId13" display="https://www.mouser.com/ProductDetail/Microchip-Technology-Micrel/MIC5211-LXYM6-TR?qs=U6T8BxXiZAWZW72McTiFRQ%3D%3D"/>
+    <hyperlink ref="H10" r:id="rId14" display="https://www.mouser.com/ProductDetail/Adafruit/328/?qs=%2Fha2pyFadujwErubcL2L61P2WtCOdI0NVdDECC%252B%2FoCOknOIs%252BWOAti9IV6ILMtMSHsGVAGjMTyxRM15aoZcNPEjv2R0X%2FExV"/>
+    <hyperlink ref="G11" r:id="rId15" display="https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KRKT/386801?s=N4IgTCBcDaIIwDYAMBaOAWMB2NKByAIiALoC%2BQA"/>
+    <hyperlink ref="H11" r:id="rId16" display="https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KRKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXsqEUEEyi4%2FkmrG730tSpETf1y5CrReP0g%3D%3D"/>
+    <hyperlink ref="G12" r:id="rId17" display="https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KSKT/386803?s=N4IgTCBcDaIIwDYAMBaOAWMAONKByAIiALoC%2BQA"/>
+    <hyperlink ref="H12" r:id="rId18" display="https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KSKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXn8t9EMk8utzJwNadB3tUNYbTGxiFNDL%252BQ%3D%3D"/>
+    <hyperlink ref="G13" r:id="rId19" display="https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C171KGKT/386799"/>
+    <hyperlink ref="H13" r:id="rId20" display="https://www.mouser.com/ProductDetail/Lite-On/LTST-C171KGKT/?qs=%2Fha2pyFadugVCX%252BfBbYHXtuidLnLhtS%252BLcjo%252B7rsZImYs2WRq48j3g%3D%3D"/>
+    <hyperlink ref="G14" r:id="rId21" display="https://www.digikey.com/en/products/detail/on-semiconductor/MBR0530T3G/1477144"/>
+    <hyperlink ref="H14" r:id="rId22" display="https://www.mouser.com/ProductDetail/ON-Semiconductor/MBR0530T3G/?qs=3JMERSakebpEmdUS6GetdQ%3D%3D"/>
+    <hyperlink ref="G15" r:id="rId23" display="https://www.digikey.com/en/products/detail/infineon-technologies/IRLML0100TRPBF/2202214?s=N4IgTCBcDaIJICUAyBZJAGAjO9AVBACgEIBiAwrgLQByAIiALoC%2BQA"/>
+    <hyperlink ref="H15" r:id="rId24" display="https://www.mouser.com/ProductDetail/Infineon-IR/IRLML0100TRPBF/?qs=%2Fha2pyFadugzSi28VWDL%252B%2Fj%2FX3doh67wE%2FvCgh7X2pqnmkMc%252Bq1ivg%3D%3D"/>
+    <hyperlink ref="H16" r:id="rId25" display="https://www.mouser.com/ProductDetail/TE-Connectivity/1825232-1/?qs=sGAEpiMZZMsqIr59i2oRcon9IvqasVjyMHmjVc2ktR8%3D"/>
+    <hyperlink ref="H17" r:id="rId26" display="https://www.mouser.com/ProductDetail/TE-Connectivity-Alcoswitch/FSMSM/?qs=sGAEpiMZZMsqIr59i2oRcuc2r3r3LjiLHQssz2WjmiQ%3D"/>
+    <hyperlink ref="G18" r:id="rId27" display="https://www.digikey.com/en/products/detail/IFSC1515AHER100M01/541-1406-1-ND/2744259?itemSeq=353770760"/>
+    <hyperlink ref="H18" r:id="rId28" display="https://www.mouser.com/ProductDetail/Vishay-Dale/IFSC1515AHER100M01/?qs=%2Fha2pyFaduhyEPNk9r%2F290OYvS9yrkIBzEVVa6IllFEq60qCq9iyWQ%3D%3D"/>
+    <hyperlink ref="H19" r:id="rId29" display="https://www.mouser.com/ProductDetail/Panasonic/EVQ-P7J01P/?qs=sGAEpiMZZMsqIr59i2oRcgbPjJcuopmxlBtPLe3n9e0%3D"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>